<commit_message>
EPBDS-6955 Generate unique names for simplified syntax of test tables
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/ExpectedInTest.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/ExpectedInTest.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="28">
   <si>
     <t>return 10.0;</t>
   </si>
@@ -34,9 +34,6 @@
     <t>10.0</t>
   </si>
   <si>
-    <t>Test doubleObj doubleObjString</t>
-  </si>
-  <si>
     <t>Method Object intObj()</t>
   </si>
   <si>
@@ -49,9 +46,6 @@
     <t>Test intObj</t>
   </si>
   <si>
-    <t>Test intObj intObjString</t>
-  </si>
-  <si>
     <t>return "10";</t>
   </si>
   <si>
@@ -61,9 +55,6 @@
     <t>Test StringObj</t>
   </si>
   <si>
-    <t>Test StringObj StringObjString</t>
-  </si>
-  <si>
     <t>return new double[] {10.0};</t>
   </si>
   <si>
@@ -91,15 +82,6 @@
     <t>Test StringObjArr</t>
   </si>
   <si>
-    <t>Test StringObjArr StringObjArrString</t>
-  </si>
-  <si>
-    <t>Test intObjArr intObjArrString</t>
-  </si>
-  <si>
-    <t>Test doubleObjArr doubleObjArrString</t>
-  </si>
-  <si>
     <t>Method Object[] doubleArr()</t>
   </si>
   <si>
@@ -116,15 +98,6 @@
   </si>
   <si>
     <t>Test StringArr</t>
-  </si>
-  <si>
-    <t>Test doubleObjArr doubleArrString</t>
-  </si>
-  <si>
-    <t>Test intObjArr intArrString</t>
-  </si>
-  <si>
-    <t>Test StringArr StringArrString</t>
   </si>
 </sst>
 </file>
@@ -463,8 +436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="125" workbookViewId="0">
-      <selection activeCell="H50" sqref="H50"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -481,7 +454,7 @@
         <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
@@ -516,10 +489,10 @@
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.2">
@@ -532,7 +505,7 @@
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D11" t="s">
         <v>4</v>
@@ -543,21 +516,21 @@
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12">
+        <v>10</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="D12">
-        <v>10</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D16" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F16" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.2">
@@ -570,7 +543,7 @@
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D18" t="s">
         <v>4</v>
@@ -581,21 +554,21 @@
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D19">
         <v>10</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D25" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F25" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.2">
@@ -608,7 +581,7 @@
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D27" t="s">
         <v>4</v>
@@ -619,7 +592,7 @@
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D28">
         <v>10</v>
@@ -630,10 +603,10 @@
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D32" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F32" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.2">
@@ -646,7 +619,7 @@
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D34" t="s">
         <v>4</v>
@@ -657,21 +630,21 @@
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D35">
         <v>10</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D39" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F39" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.2">
@@ -684,7 +657,7 @@
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D41" t="s">
         <v>4</v>
@@ -695,21 +668,21 @@
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D42">
         <v>10</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D50" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="F50" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="51" spans="2:6" x14ac:dyDescent="0.2">
@@ -722,7 +695,7 @@
     </row>
     <row r="52" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D52" t="s">
         <v>4</v>
@@ -733,7 +706,7 @@
     </row>
     <row r="53" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D53">
         <v>10</v>
@@ -744,10 +717,10 @@
     </row>
     <row r="57" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D57" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="F57" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
     </row>
     <row r="58" spans="2:6" x14ac:dyDescent="0.2">
@@ -760,7 +733,7 @@
     </row>
     <row r="59" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D59" t="s">
         <v>4</v>
@@ -771,21 +744,21 @@
     </row>
     <row r="60" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D60">
         <v>10</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="64" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D64" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F64" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="65" spans="2:6" x14ac:dyDescent="0.2">
@@ -798,7 +771,7 @@
     </row>
     <row r="66" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B66" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D66" t="s">
         <v>4</v>
@@ -809,13 +782,13 @@
     </row>
     <row r="67" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D67">
         <v>10</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>